<commit_message>
Added Geckotek plate and magnet sheet
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
   <si>
     <t>Aliexpress</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Corneria 10 Magnetic Sheets Adhesive 20 Mil Magnet</t>
+  </si>
+  <si>
+    <t>Amazon - Corneria</t>
+  </si>
+  <si>
+    <t>https://www.geckotek.co/product/geckotek-rt-build-plate-3d-printing-surface/</t>
+  </si>
+  <si>
+    <t>Geckotek RT 120x120mm</t>
   </si>
 </sst>
 </file>
@@ -276,7 +288,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +299,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -315,11 +335,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,15 +358,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -624,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,7 +669,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(D:D)</f>
-        <v>1312.93</v>
+        <v>1337.44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -659,7 +682,7 @@
       <c r="C3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -678,10 +701,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
@@ -696,16 +719,8 @@
       <c r="D8" s="2">
         <v>22</v>
       </c>
-      <c r="E8" s="1">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>11</v>
-      </c>
-      <c r="G8" s="8">
-        <f>SUM(F8:F33)</f>
-        <v>313.55</v>
-      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
@@ -720,12 +735,7 @@
       <c r="D9" s="2">
         <v>26.25</v>
       </c>
-      <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2">
-        <v>17.5</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
@@ -740,12 +750,7 @@
       <c r="D10" s="2">
         <v>28.6</v>
       </c>
-      <c r="E10" s="1">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2">
-        <v>28.6</v>
-      </c>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
@@ -760,16 +765,11 @@
       <c r="D11" s="2">
         <v>14</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>14</v>
-      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>67</v>
@@ -778,14 +778,9 @@
         <v>66</v>
       </c>
       <c r="D12" s="2">
-        <v>29.9</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
         <v>14.95</v>
       </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
@@ -800,12 +795,7 @@
       <c r="D13" s="2">
         <v>27</v>
       </c>
-      <c r="E13" s="1">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2">
-        <v>27</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
@@ -844,13 +834,7 @@
       <c r="D16" s="2">
         <v>13.9</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <f>13.9/2</f>
-        <v>6.95</v>
-      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
@@ -865,13 +849,7 @@
       <c r="D17" s="2">
         <v>41.5</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <f>41.5/2</f>
-        <v>20.75</v>
-      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
@@ -886,13 +864,7 @@
       <c r="D18" s="2">
         <v>41.7</v>
       </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2">
-        <f>27.8/2</f>
-        <v>13.9</v>
-      </c>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
@@ -907,13 +879,7 @@
       <c r="D19" s="2">
         <v>123</v>
       </c>
-      <c r="E19" s="1">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2">
-        <f>123/2</f>
-        <v>61.5</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
@@ -928,13 +894,7 @@
       <c r="D20" s="2">
         <v>87.1</v>
       </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <f>87.1/2</f>
-        <v>43.55</v>
-      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
@@ -949,13 +909,7 @@
       <c r="D21" s="2">
         <v>19.7</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <f>19.7/2</f>
-        <v>9.85</v>
-      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
@@ -970,13 +924,7 @@
       <c r="D22" s="2">
         <v>24</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <f>24/2</f>
-        <v>12</v>
-      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
@@ -991,12 +939,7 @@
       <c r="D23" s="2">
         <v>2</v>
       </c>
-      <c r="E23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2</v>
-      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
@@ -1011,9 +954,7 @@
       <c r="D24" s="2">
         <v>15.8</v>
       </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
@@ -1028,12 +969,7 @@
       <c r="D25" s="2">
         <v>4</v>
       </c>
-      <c r="E25" s="1">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2</v>
-      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
@@ -1048,12 +984,7 @@
       <c r="D26" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E26" s="1">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
@@ -1068,12 +999,7 @@
       <c r="D27" s="2">
         <v>16.350000000000001</v>
       </c>
-      <c r="E27" s="1">
-        <v>3</v>
-      </c>
-      <c r="F27" s="2">
-        <v>16.350000000000001</v>
-      </c>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
@@ -1088,12 +1014,7 @@
       <c r="D28" s="2">
         <v>6.95</v>
       </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
-        <v>6.95</v>
-      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
@@ -1108,9 +1029,7 @@
       <c r="D29" s="2">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
@@ -1125,9 +1044,7 @@
       <c r="D30" s="2">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
@@ -1142,9 +1059,7 @@
       <c r="D31" s="2">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
@@ -1159,12 +1074,7 @@
       <c r="D32" s="2">
         <v>2.5</v>
       </c>
-      <c r="E32" s="1">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2">
-        <v>2.5</v>
-      </c>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
@@ -1179,9 +1089,7 @@
       <c r="D33" s="2">
         <v>50</v>
       </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
@@ -1373,12 +1281,43 @@
       </c>
       <c r="C48" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="2">
+        <v>10.46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="2">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A7:B7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C50" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>